<commit_message>
Update Microcontroller_interfacing_BOM.xlsx to include other small components
</commit_message>
<xml_diff>
--- a/Production/Microcontroller_interfacing_BOM.xlsx
+++ b/Production/Microcontroller_interfacing_BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UCT 2022\EEE3088F Design Principles\Task\2 Design Proposal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4082895B-F111-43A8-BBC3-46DCDFB3807D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ACAA035-29B1-4E65-81C7-9E46DFD93CA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{87200DD5-525B-4095-95B5-49754A1CF272}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="44">
   <si>
     <t xml:space="preserve">Part </t>
   </si>
@@ -162,6 +162,9 @@
   </si>
   <si>
     <t>Above is using first option</t>
+  </si>
+  <si>
+    <t>Not accounted for are resistors, capacitors and diodes which are cheap</t>
   </si>
 </sst>
 </file>
@@ -571,10 +574,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACD1B5A-A6A6-488D-B415-41EF40D19B5A}">
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -812,6 +815,11 @@
         <v>42</v>
       </c>
     </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:F2"/>

</xml_diff>

<commit_message>
Update Schematic and BOM
</commit_message>
<xml_diff>
--- a/Production/Microcontroller_interfacing_BOM.xlsx
+++ b/Production/Microcontroller_interfacing_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UCT 2022\EEE3088F Design Principles\Task\Git\eee088f-group-5\Production\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0549904-38C8-4A07-A9FB-C39A25E6A0E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3941CC4-9827-45B4-93A6-409A86317919}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{87200DD5-525B-4095-95B5-49754A1CF272}"/>
+    <workbookView xWindow="14316" yWindow="1488" windowWidth="17280" windowHeight="8964" xr2:uid="{87200DD5-525B-4095-95B5-49754A1CF272}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -645,8 +645,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7ACD1B5A-A6A6-488D-B415-41EF40D19B5A}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>